<commit_message>
Analysis of both experiments: cueing and effects of blink parameters.
</commit_message>
<xml_diff>
--- a/cond-files/cond_eb2.xlsx
+++ b/cond-files/cond_eb2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\eb\eb\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F69783-7419-41B1-8A0E-8A227C6D374D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABE9CE5-820A-48B6-9404-AD0BBDA1E716}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="14020" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98:C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -915,10 +915,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -929,10 +929,10 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -940,9 +940,1120 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
         <v>1200</v>
       </c>
     </row>

</xml_diff>